<commit_message>
Output with sample footnotes
</commit_message>
<xml_diff>
--- a/clinical_study_report_summary.xlsx
+++ b/clinical_study_report_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,271 +452,91 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Table 14.1.1: Demographics and Baseline Characteristics 4</t>
+          <t>Table 1.1 Incidence of AEs by Preferred Term and System Organ Class</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(1) Table 1.1 Incidence of AEs by Preferred Term and System Organ Class | (2) System Organ Preferred Term Treatment Group 1 Treatment Group 2 | (3) Class (N=X) (N=Y) | (4) Any System Organ | (5) Class | (6) Any Preferred Term n (%) n (%) | (7) Blood and | (8) Lymphatic System | (9) Disorders | (10) Anemia n (%) n (%) | (11) Neutropenia n (%) n (%) | (12) Gastrointestinal | (13) Disorders | (14) Diarrhea n (%) n (%) | (15) Nausea n (%) n (%) | (16) Vomiting n (%) n (%) | (17) General Disorders | (18) and Administration | (19) Site Conditions | (20) Fatigue n (%) n (%) | (21) Pyrexia n (%) n (%) | (22) Nervous System | (23) Disorders | (24) Headache n (%) n (%) | (25) Dizziness n (%) n (%) | (26) Skin and | (27) Subcutaneous | (28) Tissue Disorders | (29) Rash n (%) n (%)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Table 14.1.1: Demographics and Baseline Characteristics</t>
+          <t>Table 1.2 Incidence of Serious AEs by Preferred Term and System Organ Class</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(1) AE: Adverse event | (2) Adverse events before treatment start date are not considered. | (3) Adverse events before treatment start date are not considered. | (4) AE’s also include treatment emergent events. | (5) Table 1.2 Incidence of Serious AEs by Preferred Term and System Organ Class | (6) System Organ Preferred Term Treatment Group 1 Treatment Group 2 | (7) System Organ Preferred Term Treatment Group 1 Treatment Group 2 | (8) Class (N=X) (N=Y) | (9) Any System Organ | (10) Class | (11) Class | (12) Any Preferred Term n (%) n (%) | (13) Blood and | (14) Lymphatic System | (15) Lymphatic System | (16) Disorders | (17) Anemia n (%) n (%) | (18) Neutropenia n (%) n (%) | (19) Gastrointestinal | (20) Gastrointestinal | (21) Disorders | (22) Diarrhea n (%) n (%) | (23) Nausea n (%) n (%) | (24) Vomiting n (%) n (%) | (25) General Disorders | (26) and Administration | (27) Site Conditions | (28) Site Conditions | (29) Fatigue n (%) n (%) | (30) Pyrexia n (%) n (%) | (31) Nervous System | (32) Nervous System | (33) Disorders | (34) Headache n (%) n (%) | (35) Dizziness n (%) n (%)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Table 14.1.2: Medical History</t>
+          <t>Table 1.3 Incidence of AEs Leading to Discontinuation by Preferred Term and System</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(1) Subcutaneous | (2) Tissue Disorders | (3) Tissue Disorders | (4) Rash n (%) n (%) | (5) Rash n (%) n (%) | (6) Pruritus n (%) n (%) | (7) AE: Adverse event | (8) AE: Adverse event | (9) Serious AE: Serious Adverse event | (10) Adverse events before treatment start date are not considered. | (11) AE’s also include treatment emergent events. | (12) Table 1.3 Incidence of AEs Leading to Discontinuation by Preferred Term and System | (13) Table 1.3 Incidence of AEs Leading to Discontinuation by Preferred Term and System | (14) Organ Class | (15) System Organ Preferred Term Treatment Group 1 Treatment Group 2 | (16) Class (N=X) (N=Y) | (17) Any System Organ | (18) Class | (19) Any Preferred Term n (%) n (%) | (20) Blood and | (21) Blood and | (22) Lymphatic System | (23) Disorders | (24) Disorders | (25) Anemia n (%) n (%) | (26) Neutropenia n (%) n (%) | (27) Gastrointestinal | (28) Disorders | (29) Diarrhea n (%) n (%) | (30) Nausea n (%) n (%) | (31) Vomiting n (%) n (%) | (32) General Disorders | (33) General Disorders | (34) and Administration | (35) Site Conditions | (36) Site Conditions | (37) Fatigue n (%) n (%) | (38) Fatigue n (%) n (%) | (39) Pyrexia n (%) n (%)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Table 14.2.1: Primary Efficacy Analysis - Change from Baseline at Week 12</t>
+          <t>Table 2.1 Summary of Laboratory Values - Hematology</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(1) Nervous System | (2) Disorders | (3) Headache n (%) n (%) | (4) Headache n (%) n (%) | (5) Dizziness n (%) n (%) | (6) Skin and | (7) Subcutaneous | (8) Subcutaneous | (9) Tissue Disorders | (10) Rash n (%) n (%) | (11) Pruritus n (%) n (%) | (12) Pruritus n (%) n (%) | (13) AE: Adverse event | (14) Adverse events leading to discontinuation | (15) Adverse events leading to discontinuation | (16) Adverse events before treatment start date are not considered. | (17) AE’s also include treatment emergent events. | (18) Table 2.1 Summary of Laboratory Values - Hematology | (19) Parameter Statistic Treatment Group 1 Treatment Group 2 | (20) (N=X) (N=Y) | (21) (N=X) (N=Y) | (22) Hemoglobin (g/dL) N | (23) Hemoglobin (g/dL) N | (24) Mean (SD) | (25) Median | (26) Min, Max | (27) White Blood Cell N | (28) Count (x10^9/L) | (29) Count (x10^9/L) | (30) Count (x10^9/L) | (31) Mean (SD) | (32) Mean (SD) | (33) Median | (34) Min, Max | (35) Platelet Count N | (36) (x10^9/L) | (37) (x10^9/L) | (38) Mean (SD) | (39) Mean (SD)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Table 14.3.1: Treatment-Emergent Adverse Events by System Organ Class and Preferred Term</t>
+          <t>Table 2.2 Summary of Laboratory Values - Chemistry</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>(1) Median | (2) Min, Max | (3) Summary statistics for laboratory parameters. | (4) Values presented at baseline and each post-baseline visit. | (5) Values presented at baseline and each post-baseline visit. | (6) Table 2.2 Summary of Laboratory Values - Chemistry | (7) Table 2.2 Summary of Laboratory Values - Chemistry | (8) Parameter Statistic Treatment Group 1 Treatment Group 2 | (9) (N=X) (N=Y) | (10) Alanine N | (11) Aminotransferase | (12) (U/L) | (13) Mean (SD) | (14) Median | (15) Min, Max | (16) Aspartate N | (17) Aminotransferase | (18) (U/L) | (19) Mean (SD) | (20) Median | (21) Min, Max | (22) Total Bilirubin N | (23) (µmol/L) | (24) Mean (SD) | (25) Median | (26) Min, Max | (27) Creatinine (µmol/L) N | (28) Mean (SD) | (29) Mean (SD) | (30) Median</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Table 14.3.2: Summary of Laboratory Test Results - Change from Baseline</t>
+          <t>Table 2.3 Summary of Laboratory Values - Urinalysis</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>11</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Table 14.3.3: Summary of Vital Signs - Change from Baseline</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>14</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Figure 14.2.1: Primary Endpoint Over Time</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Note: Error bars represent standard error of the mean.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>15</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Figure 14.2.2: Subgroup Analysis of Primary Endpoint</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>16</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Figure 14.3.1: Adverse Events by System Organ Class</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>17</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Listing 16.2.1: Patient Disposition</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Note: This listing provides patient disposition information for all randomized patients.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>18</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Listing 16.2.2: Protocol Deviations</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>19</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Listing 16.2.3: Patients Excluded from Analysis Populations</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>20</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Listing 16.2.4: Demographic Data</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>21</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Listing 16.2.5: Concomitant Medications</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>22</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Listing 16.2.6: Individual Efficacy Response Data</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>23</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Listing 16.2.7: Adverse Event Listings</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>24</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Listing 16.2.8: Individual Laboratory Measurements</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>(1) (N=X) (N=Y) | (2) Protein N | (3) (Qualitative) | (4) Negative n (%) n (%) | (5) Trace | (6) Figure 2.2 Kaplan-Meier Plot for Time to Discontinuation Due to Adverse Event | (7) 1.0 +-----------------------------------------------------+ | (8) | | | (9) | | | (10) | +---------Treatment Group 1 | | (11) | / | | (12) | / | | (13) | / | | (14) | / | | (15) | +-----------Treatment Group 2 | | (16) | / | | (17) | / | | (18) | / | | (19) 0.0 +-----------------------------------------------------+ | (20) 0.0 +-----------------------------------------------------+ | (21) 0 Time (Days) Max Time | (22) X-axis: Time (Days) | (23) X-axis: Time (Days) | (24) Y-axis: Probability of No Discontinuation | (25) Description: Kaplan-Meier plot showing the probability of not | (26) discontinuing due to an adverse event over time for each treatment | (27) group. | (28) group. | (29) Figure 2.3 Kaplan-Meier Plot for Overall Survival | (30) 1.0 +-----------------------------------------------------+ | (31) 1.0 +-----------------------------------------------------+ | (32) | | | (33) | | | (34) | +---------Treatment Group 1 | | (35) | / | | (36) | / | | (37) | / | | (38) | / | | (39) | / |</t>
         </is>
       </c>
     </row>

</xml_diff>